<commit_message>
[CART] ajout les cas de test pour fonc CART
</commit_message>
<xml_diff>
--- a/ressources/AUSY_Cas_de_test.xlsx
+++ b/ressources/AUSY_Cas_de_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33698\PycharmProjects\Robotframework\Test_Ausy\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F13DEA6-F0DD-425C-A593-780F4F05677E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D04B20-6E32-4B42-9D51-EFBF177F19F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AUTH_LOG_01_Valid" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,10 @@
     <sheet name="AUTH_LOG_04_Login_Close" sheetId="4" r:id="rId4"/>
     <sheet name="AUTH_SIGN_01_New_User_Valid" sheetId="6" r:id="rId5"/>
     <sheet name="AUTH_SIGN_02_New_User_Exist" sheetId="7" r:id="rId6"/>
-    <sheet name="CART_01_Annuler_OrderPlace" sheetId="5" r:id="rId7"/>
+    <sheet name="AUTH_SIGN_03_Invalid_InputBlank" sheetId="8" r:id="rId7"/>
+    <sheet name="CART_01_Annuler_PlaceOrder" sheetId="5" r:id="rId8"/>
+    <sheet name="CART_02_PlaceOrder_Valide" sheetId="9" r:id="rId9"/>
+    <sheet name="CART_03_PlaceOrder_Input_Blank" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="120">
   <si>
     <t xml:space="preserve">En tant que l'utilisateur de l'application Product Store (SP), </t>
   </si>
@@ -202,9 +205,6 @@
   </si>
   <si>
     <t>Click bouton "Close" dans modal</t>
-  </si>
-  <si>
-    <t>CART_01_Annuler_OrderPlace</t>
   </si>
   <si>
     <t>AUTH_LOG_01_Login_User_Valid</t>
@@ -320,6 +320,109 @@
   </si>
   <si>
     <t>Modal "Sign up" ferme</t>
+  </si>
+  <si>
+    <t>AUTH SIGN_03</t>
+  </si>
+  <si>
+    <t>je peux aller au page "Sign_Up" pour m'inscrire, si je ne renseigne pas username ni password ou aucun les deux</t>
+  </si>
+  <si>
+    <t>l'application va me donner un message d'erreur "Please fill out Username and Password."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User renseigne 
+- soit &lt;username&gt;, sans &lt;password&gt;
+- soit &lt;password&gt;, sans &lt;username&gt;
+- aucun les deux
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;username&gt;  existe dans SP</t>
+  </si>
+  <si>
+    <t>Popup d'erreur d'insciption affiche "Please fill out Username and Password."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+- input Username est rempli
+- input Password est rempli
+- Username et password sont vide</t>
+  </si>
+  <si>
+    <t>AUTH_SIGN_03_Invalid_InputBlank</t>
+  </si>
+  <si>
+    <t>CART_01_Annuler_PlaceOrder</t>
+  </si>
+  <si>
+    <t>CART_02_PlaceOrder_Valide</t>
+  </si>
+  <si>
+    <t>CART_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">je renseigne les infos de mon order et je le confirme </t>
+  </si>
+  <si>
+    <t>l'app me donnera un message contenant mes infos saisies</t>
+  </si>
+  <si>
+    <t>donnée du card: name, city, country, card_number, month, year</t>
+  </si>
+  <si>
+    <t>Modal "Place order" affiche</t>
+  </si>
+  <si>
+    <t>Les données saisies sont affichées dans les champs</t>
+  </si>
+  <si>
+    <t>Click bouton "Purchase" dans modal</t>
+  </si>
+  <si>
+    <t>Click bouton "OK" du popup</t>
+  </si>
+  <si>
+    <t>Popup disparait</t>
+  </si>
+  <si>
+    <t>User renseigne les données
+- Name
+- City
+- Country
+- Credit card
+- Month
+- Year</t>
+  </si>
+  <si>
+    <t>Popup de confirmation de purchase affiche
+- Name
+- Credit card
+- Amount: 0</t>
+  </si>
+  <si>
+    <t>CART_03_PlaceOrder_Input_Blank</t>
+  </si>
+  <si>
+    <t>CART_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant que l'utilisateur de l'application Product Store (SP),  je vais au page Cart, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">je ne renseigne pas les infos et je le confirme </t>
+  </si>
+  <si>
+    <t>l'app me donnera un message error "Please fill out Name and Creditcard."</t>
+  </si>
+  <si>
+    <t>Popup affiche message d'erreur "Please fill out Name and Creditcard."</t>
+  </si>
+  <si>
+    <t>Fermer modal "Place Order" en cliquant bouton [X]</t>
+  </si>
+  <si>
+    <t>Modal "Place order" disparait</t>
   </si>
 </sst>
 </file>
@@ -747,10 +850,10 @@
   <sheetData>
     <row r="1" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -945,14 +1048,14 @@
         <v>24</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
@@ -1004,6 +1107,251 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783E6149-C2C0-48B1-A882-EA1AC6229F3B}">
+  <dimension ref="A1:M20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.08984375" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="10.90625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4"/>
+      <c r="B13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+    </row>
+    <row r="14" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+    </row>
+    <row r="15" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+    </row>
+    <row r="18" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+    </row>
+    <row r="19" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+    </row>
+    <row r="20" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="G20:M20"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="G19:M19"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="G17:M17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="G18:M18"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="G13:M13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:F15"/>
+    <mergeCell ref="G14:M15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="G16:M16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M19"/>
@@ -1020,10 +1368,10 @@
   <sheetData>
     <row r="1" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1268,7 +1616,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1278,10 +1628,10 @@
   <sheetData>
     <row r="1" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1469,10 +1819,10 @@
   <sheetData>
     <row r="1" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1706,10 +2056,10 @@
   <sheetData>
     <row r="1" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1717,12 +2067,12 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1745,7 +2095,7 @@
     </row>
     <row r="8" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1790,14 +2140,14 @@
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -1883,14 +2233,14 @@
         <v>21</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
@@ -1904,14 +2254,14 @@
         <v>24</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
@@ -1925,14 +2275,14 @@
         <v>36</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -1943,10 +2293,10 @@
     </row>
     <row r="23" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1962,10 +2312,10 @@
     </row>
     <row r="24" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1981,10 +2331,10 @@
     </row>
     <row r="25" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -2000,7 +2350,7 @@
     </row>
     <row r="26" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>25</v>
@@ -2019,10 +2369,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="G22:M22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="G23:M23"/>
-    <mergeCell ref="B25:F25"/>
     <mergeCell ref="G25:M25"/>
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="G26:M26"/>
@@ -2036,13 +2382,17 @@
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="G21:M21"/>
     <mergeCell ref="B22:F22"/>
+    <mergeCell ref="G22:M22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="G23:M23"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="G17:M17"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="G14:M14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:F16"/>
     <mergeCell ref="G15:M16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="G17:M17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2053,8 +2403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{291B2F49-3C43-42DB-84E4-6D291C877DF9}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22:M22"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2065,10 +2415,10 @@
   <sheetData>
     <row r="1" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2076,17 +2426,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2104,7 +2454,7 @@
     </row>
     <row r="8" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2149,14 +2499,14 @@
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -2242,14 +2592,14 @@
         <v>21</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
@@ -2263,14 +2613,14 @@
         <v>24</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
@@ -2284,14 +2634,14 @@
         <v>24</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -2332,13 +2682,13 @@
     <mergeCell ref="G20:M20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="G21:M21"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="G17:M17"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="G14:M14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:F16"/>
     <mergeCell ref="G15:M16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="G17:M17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2346,11 +2696,255 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A127D728-C309-4421-9AB7-2F26233200E0}">
+  <dimension ref="A1:M20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.08984375" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="10.90625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4"/>
+      <c r="B13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+    </row>
+    <row r="14" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+    </row>
+    <row r="15" spans="1:13" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="1:13" ht="62" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+    </row>
+    <row r="18" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+    </row>
+    <row r="19" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+    </row>
+    <row r="20" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="G16:M16"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="G13:M13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:F15"/>
+    <mergeCell ref="G14:M15"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="G19:M19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="G20:M20"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="G17:M17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="G18:M18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D77E102C-2DBF-4DB9-AFF0-2928E1D2FEAD}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2364,7 +2958,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2555,4 +3149,284 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A534B934-28C0-41C7-95D8-FFAA26536051}">
+  <dimension ref="A1:M22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.08984375" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="10.90625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4"/>
+      <c r="B13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+    </row>
+    <row r="14" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+    </row>
+    <row r="15" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+    </row>
+    <row r="18" spans="1:13" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+    </row>
+    <row r="19" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="1:13" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+    </row>
+    <row r="21" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+    </row>
+    <row r="22" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="G19:M20"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="G22:M22"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="G21:M21"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:F18"/>
+    <mergeCell ref="G17:M18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:F20"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="G13:M13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:F15"/>
+    <mergeCell ref="G14:M15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="G16:M16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>